<commit_message>
some fixs + another bug
</commit_message>
<xml_diff>
--- a/game faults and bugs.xlsx
+++ b/game faults and bugs.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colin\Desktop\Development-Project-communal (1)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61367F28-D649-49F5-B684-8F9A4F35FC50}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="132" windowWidth="20112" windowHeight="7932" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Small cursor displaying on spash screen</t>
   </si>
@@ -81,9 +75,6 @@
   </si>
   <si>
     <t xml:space="preserve">The location of each answer button needs to be randomised within each question. This is vital because of how the data is retrived from the database, the correct answer will always be first </t>
-  </si>
-  <si>
-    <t>aaron</t>
   </si>
   <si>
     <t>Notes</t>
@@ -119,12 +110,34 @@
     <t>on initiate if the game cannot hit the server nothing happens from user perspective
 Minimum solution: error message to user, exit program
 Best solution: game loads from locally stored data</t>
+  </si>
+  <si>
+    <t>It is possible to make multiple answer selections</t>
+  </si>
+  <si>
+    <t>after a user makes selects an answer they need to blocked from making another selection</t>
+  </si>
+  <si>
+    <t>added a clicked bool that is checked before a user makes a selection. It is set when they make a selection and reset when the next question is shown.</t>
+  </si>
+  <si>
+    <t>col</t>
+  </si>
+  <si>
+    <t>added color to answer button on user selection. 
+Added time delay so users can see it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ramdomised where buttons are </t>
+  </si>
+  <si>
+    <t>duplications of questions are bein shown within the same game</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -199,7 +212,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -235,7 +248,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -307,7 +320,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,26 +353,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -392,23 +388,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -584,24 +563,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.44140625" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -615,7 +594,7 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -626,13 +605,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
@@ -643,15 +622,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="100.9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -662,7 +641,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="43.15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -675,45 +654,76 @@
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D8" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>34</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="2" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>27</v>
+      <c r="C11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -724,24 +734,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2 found bugs
Small bugs found, text partially showing on menu and question without answer buttons
</commit_message>
<xml_diff>
--- a/game faults and bugs.xlsx
+++ b/game faults and bugs.xlsx
@@ -1,28 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\Games\Uni\Development-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PeacheyMacbook/Google Drive/Uni/Development-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE32047-BED0-4211-91BA-59E185156911}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="30580" windowHeight="16160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>Small cursor displaying on spash screen</t>
   </si>
@@ -159,12 +163,27 @@
   </si>
   <si>
     <t>Disagree. You'll see the button outlines if you do this and if you change the button to transparent the ripple effect doesn't show. I did implement this at first and it looked horrible.</t>
+  </si>
+  <si>
+    <t>Can see username behind 'New Game' on menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">After log in, the username text can be partially seen behind the 'New Game' text. </t>
+  </si>
+  <si>
+    <t>Lord of the Rings question has no answer buttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every other question but this one question has no answer buttons present. </t>
+  </si>
+  <si>
+    <t>Aaron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -239,7 +258,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -275,7 +294,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -293,6 +312,80 @@
         <a:xfrm>
           <a:off x="11477625" y="120015"/>
           <a:ext cx="2394295" cy="1601899"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="26545" b="33210"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12407900" y="9359899"/>
+          <a:ext cx="1663700" cy="1193801"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127001</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:srcRect b="63604"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14097000" y="9918735"/>
+          <a:ext cx="1968500" cy="1257266"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -350,9 +443,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -380,31 +473,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -432,23 +508,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -624,24 +683,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="36.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="45.5" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -658,7 +717,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -675,7 +734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -686,7 +745,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -697,7 +756,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -711,7 +770,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -722,7 +781,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -733,7 +792,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -747,7 +806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -761,7 +820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -772,7 +831,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -789,7 +848,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
@@ -803,9 +862,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -816,24 +897,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>